<commit_message>
added dtwin fields to excel reporting templates and also added colors to increase visual aid
</commit_message>
<xml_diff>
--- a/excel_reporting_templates/IotSensorData-2.0.0-schema-reporting_template.xlsx
+++ b/excel_reporting_templates/IotSensorData-2.0.0-schema-reporting_template.xlsx
@@ -8,9 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="semantic_aspect_model_schema" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="possible_values" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="description" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="metadata" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="description" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="metadata" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,8 +27,11 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -38,12 +40,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00B7DEE8"/>
+        <bgColor rgb="00B7DEE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEB9C"/>
+        <bgColor rgb="00FFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFDE9"/>
+        <bgColor rgb="00FFFDE9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C4D79B"/>
+        <bgColor rgb="00C4D79B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="0000FF00"/>
         <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,14 +77,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,71 +481,95 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.8" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="50" customWidth="1" min="4" max="4"/>
-    <col width="50" customWidth="1" min="5" max="5"/>
-    <col width="39.6" customWidth="1" min="6" max="6"/>
-    <col width="36" customWidth="1" min="7" max="7"/>
+    <col width="8.4" customWidth="1" min="1" max="1"/>
+    <col width="14.4" customWidth="1" min="2" max="2"/>
+    <col width="4.8" customWidth="1" min="3" max="3"/>
+    <col width="14.4" customWidth="1" min="4" max="4"/>
+    <col width="10.8" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
     <col width="50" customWidth="1" min="8" max="8"/>
     <col width="50" customWidth="1" min="9" max="9"/>
-    <col width="50" customWidth="1" min="10" max="10"/>
-    <col width="46.8" customWidth="1" min="11" max="11"/>
+    <col width="39.6" customWidth="1" min="10" max="10"/>
+    <col width="36" customWidth="1" min="11" max="11"/>
+    <col width="50" customWidth="1" min="12" max="12"/>
+    <col width="50" customWidth="1" min="13" max="13"/>
+    <col width="50" customWidth="1" min="14" max="14"/>
+    <col width="46.8" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ownerID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>serialNumber</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
           <t>catenaXId</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorGeoLocation_latitude</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorGeoLocation_longitude</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorGeoLocation_altitude</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorGeoLocation_geoDataTimestamp</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_batteryLevel</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_timestamp</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorData[0]_sensorType</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorData[0]_sensorValue</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorData[0]_sensorUnit</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="2" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_transmissionMethod</t>
         </is>
@@ -514,25 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,161 +599,256 @@
     <col width="17" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="22" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Legends</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="n"/>
+      <c r="C1" s="4" t="n"/>
+    </row>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>1. Columns highlighted in green in the 'semantic_aspect_model_schema' sheet are required fields.</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="n"/>
+      <c r="C2" s="4" t="n"/>
+    </row>
+    <row r="3" ht="30" customHeight="1">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>2. Columns highlighted in olive green are digital twin fields.</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="n"/>
+      <c r="C3" s="4" t="n"/>
+    </row>
+    <row r="4" ht="22" customHeight="1">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Column Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C4" s="5" t="inlineStr">
         <is>
           <t>Possible Values</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>ownerID</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>Digital Twin Field: ownerID</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>serialNumber</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>Digital Twin Field: serialNumber</t>
+        </is>
+      </c>
+      <c r="C6" s="7" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>Digital Twin Field: type</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>Digital Twin Field: manufacturer</t>
+        </is>
+      </c>
+      <c r="C8" s="7" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>catenaXId</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>The fully anonymous Catena-X ID of the asset, valid for the Catena-X dataspace.</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="C9" s="6" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorGeoLocation_latitude</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>The angle between zenith and a plane parallel to the equator.</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="C10" s="7" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorGeoLocation_longitude</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>Geographic coordinate that specifies the east-west position of a point on the Earth's surface.</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="C11" s="6" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorGeoLocation_altitude</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Antenna Altitude above/below mean-sea-level (geoid).</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="C12" s="7" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorGeoLocation_geoDataTimestamp</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>The timestamp of the latest sensor reading of the geo data.</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="C13" s="6" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_batteryLevel</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B14" s="7" t="inlineStr">
         <is>
           <t>The battery level displays how much charge of the battery has been left.</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="C14" s="7" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_timestamp</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B15" s="6" t="inlineStr">
         <is>
           <t>The timestamp of the latest sensor reading.</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="C15" s="6" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorData[0]_sensorType</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B16" s="7" t="inlineStr">
         <is>
           <t>Different types of sensors that are commonly used in various applications, measuring one of the physical properties like Temperature, Pressure,  Resistance, Shock, Conduction, Heat Transfer etc.</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="C16" s="7" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorData[0]_sensorValue</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B17" s="6" t="inlineStr">
         <is>
           <t>The measured value of the sensor type.</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="C17" s="6" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_sensorData[0]_sensorUnit</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B18" s="7" t="inlineStr">
         <is>
           <t>Describes a Property containing a reference to one of the units in the Unit Catalog.</t>
         </is>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="C18" s="7" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
         <is>
           <t>sensorRuntimeData[0]_transmissionMethod</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B19" s="6" t="inlineStr">
         <is>
           <t>The method under which the sensing data is transmitted from the source to the remote node.</t>
         </is>
       </c>
+      <c r="C19" s="6" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -716,12 +865,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Key</t>
+          <t>key</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>value</t>
         </is>
       </c>
     </row>

</xml_diff>